<commit_message>
Updating sample spreadsheet to have an ARK column, fixing null record id (DM-30)
</commit_message>
<xml_diff>
--- a/WebContent/files/conversion_demo.xlsx
+++ b/WebContent/files/conversion_demo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="1876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2570" uniqueCount="1881">
   <si>
     <t>text</t>
   </si>
@@ -5623,9 +5623,6 @@
     <t>ARK</t>
   </si>
   <si>
-    <t>http://library.ucsd.edu/ark:/20775/bb1234567x</t>
-  </si>
-  <si>
     <t>foo.jpg</t>
   </si>
   <si>
@@ -5648,6 +5645,24 @@
   </si>
   <si>
     <t>Wall text</t>
+  </si>
+  <si>
+    <t>http://library.ucsd.edu/ark:/20775/zz00000011</t>
+  </si>
+  <si>
+    <t>http://library.ucsd.edu/ark:/20775/zz00000022</t>
+  </si>
+  <si>
+    <t>http://library.ucsd.edu/ark:/20775/zz00000033</t>
+  </si>
+  <si>
+    <t>http://library.ucsd.edu/ark:/20775/zz00000044</t>
+  </si>
+  <si>
+    <t>http://library.ucsd.edu/ark:/20775/zz00000055</t>
+  </si>
+  <si>
+    <t>http://library.ucsd.edu/ark:/20775/zz00000066</t>
   </si>
 </sst>
 </file>
@@ -6202,7 +6217,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -6252,6 +6267,18 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6321,7 +6348,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="67">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -6353,6 +6380,12 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -6361,6 +6394,12 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="48"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -73691,6 +73730,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="37.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
@@ -76210,6 +76250,9 @@
       </c>
     </row>
     <row r="2" spans="1:635" s="17" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A2" s="17" t="s">
+        <v>1875</v>
+      </c>
       <c r="B2" s="26" t="s">
         <v>1186</v>
       </c>
@@ -78074,7 +78117,12 @@
       </c>
     </row>
     <row r="3" spans="1:635" s="17" customFormat="1">
-      <c r="B3" s="26"/>
+      <c r="A3" s="17" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>1186</v>
+      </c>
       <c r="C3" s="27" t="s">
         <v>1782</v>
       </c>
@@ -79916,6 +79964,9 @@
       <c r="XI3" s="26"/>
     </row>
     <row r="4" spans="1:635" s="22" customFormat="1">
+      <c r="A4" s="17" t="s">
+        <v>1876</v>
+      </c>
       <c r="B4" s="22">
         <v>556</v>
       </c>
@@ -79957,6 +80008,9 @@
       </c>
     </row>
     <row r="5" spans="1:635" s="22" customFormat="1">
+      <c r="A5" s="17" t="s">
+        <v>1877</v>
+      </c>
       <c r="B5" s="22">
         <v>557</v>
       </c>
@@ -79995,6 +80049,9 @@
       </c>
     </row>
     <row r="6" spans="1:635" s="22" customFormat="1">
+      <c r="A6" s="17" t="s">
+        <v>1877</v>
+      </c>
       <c r="B6" s="22">
         <v>557</v>
       </c>
@@ -80011,6 +80068,9 @@
       <c r="WU6" s="24"/>
     </row>
     <row r="7" spans="1:635" s="22" customFormat="1">
+      <c r="A7" s="17" t="s">
+        <v>1877</v>
+      </c>
       <c r="B7" s="22">
         <v>557</v>
       </c>
@@ -80027,6 +80087,9 @@
       <c r="WU7" s="24"/>
     </row>
     <row r="8" spans="1:635" s="22" customFormat="1">
+      <c r="A8" s="17" t="s">
+        <v>1878</v>
+      </c>
       <c r="B8" s="22">
         <v>557</v>
       </c>
@@ -80043,6 +80106,9 @@
       <c r="WU8" s="24"/>
     </row>
     <row r="9" spans="1:635" s="22" customFormat="1">
+      <c r="A9" s="17" t="s">
+        <v>1879</v>
+      </c>
       <c r="B9" s="22">
         <v>558</v>
       </c>
@@ -80085,8 +80151,8 @@
       </c>
     </row>
     <row r="10" spans="1:635">
-      <c r="A10" t="s">
-        <v>1867</v>
+      <c r="A10" s="17" t="s">
+        <v>1880</v>
       </c>
       <c r="B10" s="22">
         <v>123</v>
@@ -80095,7 +80161,7 @@
         <v>1781</v>
       </c>
       <c r="D10" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="E10" t="s">
         <v>1189</v>
@@ -80104,13 +80170,13 @@
         <v>1853</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="AA10" s="2"/>
     </row>
     <row r="11" spans="1:635">
-      <c r="A11" t="s">
-        <v>1867</v>
+      <c r="A11" s="17" t="s">
+        <v>1880</v>
       </c>
       <c r="B11" s="22">
         <v>123</v>
@@ -80119,19 +80185,19 @@
         <v>1782</v>
       </c>
       <c r="D11" t="s">
+        <v>1869</v>
+      </c>
+      <c r="E11" t="s">
         <v>1870</v>
       </c>
-      <c r="E11" t="s">
+      <c r="J11" s="39" t="s">
         <v>1871</v>
       </c>
-      <c r="J11" s="39" t="s">
-        <v>1872</v>
-      </c>
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:635">
-      <c r="A12" t="s">
-        <v>1867</v>
+      <c r="A12" s="17" t="s">
+        <v>1880</v>
       </c>
       <c r="B12" s="22">
         <v>123</v>
@@ -80140,13 +80206,13 @@
         <v>1782</v>
       </c>
       <c r="D12" t="s">
+        <v>1872</v>
+      </c>
+      <c r="E12" t="s">
         <v>1873</v>
       </c>
-      <c r="E12" t="s">
+      <c r="J12" s="39" t="s">
         <v>1874</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>1875</v>
       </c>
       <c r="AA12" s="2"/>
     </row>

</xml_diff>